<commit_message>
actualizacion carta gantt y evidencias
</commit_message>
<xml_diff>
--- a/fase_1/evidencias_grupales/Diagrama de Gantt CAPSTONE NFC.xlsx
+++ b/fase_1/evidencias_grupales/Diagrama de Gantt CAPSTONE NFC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967F1B41-062A-4653-8042-9654ABB6993F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6180539F-2E1C-4833-929B-4623BE9CCE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1401,6 +1401,24 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="171" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1412,24 +1430,6 @@
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2041,9 +2041,9 @@
   </sheetPr>
   <dimension ref="A1:DP56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2059,12 +2059,14 @@
     <col min="9" max="14" width="3.140625" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" customWidth="1"/>
     <col min="16" max="21" width="3.140625" customWidth="1"/>
-    <col min="22" max="22" width="6.5703125" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" customWidth="1"/>
     <col min="23" max="28" width="3.140625" customWidth="1"/>
-    <col min="29" max="29" width="6.85546875" customWidth="1"/>
-    <col min="30" max="35" width="3.140625" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" customWidth="1"/>
+    <col min="30" max="34" width="3.140625" customWidth="1"/>
+    <col min="35" max="35" width="11.42578125" customWidth="1"/>
     <col min="36" max="36" width="6.28515625" customWidth="1"/>
-    <col min="37" max="42" width="3.140625" customWidth="1"/>
+    <col min="37" max="41" width="3.140625" customWidth="1"/>
+    <col min="42" max="42" width="12.85546875" customWidth="1"/>
     <col min="43" max="43" width="6.140625" customWidth="1"/>
     <col min="44" max="49" width="3.140625" customWidth="1"/>
     <col min="50" max="50" width="8.5703125" customWidth="1"/>
@@ -2118,10 +2120,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="100"/>
-      <c r="E3" s="98">
+      <c r="E3" s="104">
         <v>45531</v>
       </c>
-      <c r="F3" s="98"/>
+      <c r="F3" s="104"/>
     </row>
     <row r="4" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
@@ -2134,166 +2136,166 @@
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="95">
+      <c r="I4" s="101">
         <f>I5</f>
         <v>45530</v>
       </c>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="95">
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="101">
         <f>P5</f>
         <v>45537</v>
       </c>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="96"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="96"/>
-      <c r="U4" s="96"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="95">
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="103"/>
+      <c r="W4" s="101">
         <f>W5</f>
         <v>45544</v>
       </c>
-      <c r="X4" s="96"/>
-      <c r="Y4" s="96"/>
-      <c r="Z4" s="96"/>
-      <c r="AA4" s="96"/>
-      <c r="AB4" s="96"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="95">
+      <c r="X4" s="102"/>
+      <c r="Y4" s="102"/>
+      <c r="Z4" s="102"/>
+      <c r="AA4" s="102"/>
+      <c r="AB4" s="102"/>
+      <c r="AC4" s="103"/>
+      <c r="AD4" s="101">
         <f>AD5</f>
         <v>45551</v>
       </c>
-      <c r="AE4" s="96"/>
-      <c r="AF4" s="96"/>
-      <c r="AG4" s="96"/>
-      <c r="AH4" s="96"/>
-      <c r="AI4" s="96"/>
-      <c r="AJ4" s="97"/>
-      <c r="AK4" s="95">
+      <c r="AE4" s="102"/>
+      <c r="AF4" s="102"/>
+      <c r="AG4" s="102"/>
+      <c r="AH4" s="102"/>
+      <c r="AI4" s="102"/>
+      <c r="AJ4" s="103"/>
+      <c r="AK4" s="101">
         <f>AK5</f>
         <v>45558</v>
       </c>
-      <c r="AL4" s="96"/>
-      <c r="AM4" s="96"/>
-      <c r="AN4" s="96"/>
-      <c r="AO4" s="96"/>
-      <c r="AP4" s="96"/>
-      <c r="AQ4" s="97"/>
-      <c r="AR4" s="95">
+      <c r="AL4" s="102"/>
+      <c r="AM4" s="102"/>
+      <c r="AN4" s="102"/>
+      <c r="AO4" s="102"/>
+      <c r="AP4" s="102"/>
+      <c r="AQ4" s="103"/>
+      <c r="AR4" s="101">
         <f>AR5</f>
         <v>45565</v>
       </c>
-      <c r="AS4" s="96"/>
-      <c r="AT4" s="96"/>
-      <c r="AU4" s="96"/>
-      <c r="AV4" s="96"/>
-      <c r="AW4" s="96"/>
-      <c r="AX4" s="97"/>
-      <c r="AY4" s="95">
+      <c r="AS4" s="102"/>
+      <c r="AT4" s="102"/>
+      <c r="AU4" s="102"/>
+      <c r="AV4" s="102"/>
+      <c r="AW4" s="102"/>
+      <c r="AX4" s="103"/>
+      <c r="AY4" s="101">
         <f>AY5</f>
         <v>45572</v>
       </c>
-      <c r="AZ4" s="96"/>
-      <c r="BA4" s="96"/>
-      <c r="BB4" s="96"/>
-      <c r="BC4" s="96"/>
-      <c r="BD4" s="96"/>
-      <c r="BE4" s="97"/>
-      <c r="BF4" s="95">
+      <c r="AZ4" s="102"/>
+      <c r="BA4" s="102"/>
+      <c r="BB4" s="102"/>
+      <c r="BC4" s="102"/>
+      <c r="BD4" s="102"/>
+      <c r="BE4" s="103"/>
+      <c r="BF4" s="101">
         <f>BF5</f>
         <v>45579</v>
       </c>
-      <c r="BG4" s="96"/>
-      <c r="BH4" s="96"/>
-      <c r="BI4" s="96"/>
-      <c r="BJ4" s="96"/>
-      <c r="BK4" s="96"/>
-      <c r="BL4" s="97"/>
-      <c r="BM4" s="95">
+      <c r="BG4" s="102"/>
+      <c r="BH4" s="102"/>
+      <c r="BI4" s="102"/>
+      <c r="BJ4" s="102"/>
+      <c r="BK4" s="102"/>
+      <c r="BL4" s="103"/>
+      <c r="BM4" s="101">
         <f t="shared" ref="BM4" si="0">BM5</f>
         <v>45586</v>
       </c>
-      <c r="BN4" s="96"/>
-      <c r="BO4" s="96"/>
-      <c r="BP4" s="96"/>
-      <c r="BQ4" s="96"/>
-      <c r="BR4" s="96"/>
-      <c r="BS4" s="97"/>
-      <c r="BT4" s="95">
+      <c r="BN4" s="102"/>
+      <c r="BO4" s="102"/>
+      <c r="BP4" s="102"/>
+      <c r="BQ4" s="102"/>
+      <c r="BR4" s="102"/>
+      <c r="BS4" s="103"/>
+      <c r="BT4" s="101">
         <f t="shared" ref="BT4" si="1">BT5</f>
         <v>45593</v>
       </c>
-      <c r="BU4" s="96"/>
-      <c r="BV4" s="96"/>
-      <c r="BW4" s="96"/>
-      <c r="BX4" s="96"/>
-      <c r="BY4" s="96"/>
-      <c r="BZ4" s="97"/>
-      <c r="CA4" s="95">
+      <c r="BU4" s="102"/>
+      <c r="BV4" s="102"/>
+      <c r="BW4" s="102"/>
+      <c r="BX4" s="102"/>
+      <c r="BY4" s="102"/>
+      <c r="BZ4" s="103"/>
+      <c r="CA4" s="101">
         <f t="shared" ref="CA4" si="2">CA5</f>
         <v>45600</v>
       </c>
-      <c r="CB4" s="96"/>
-      <c r="CC4" s="96"/>
-      <c r="CD4" s="96"/>
-      <c r="CE4" s="96"/>
-      <c r="CF4" s="96"/>
-      <c r="CG4" s="97"/>
-      <c r="CH4" s="95">
+      <c r="CB4" s="102"/>
+      <c r="CC4" s="102"/>
+      <c r="CD4" s="102"/>
+      <c r="CE4" s="102"/>
+      <c r="CF4" s="102"/>
+      <c r="CG4" s="103"/>
+      <c r="CH4" s="101">
         <f t="shared" ref="CH4" si="3">CH5</f>
         <v>45607</v>
       </c>
-      <c r="CI4" s="96"/>
-      <c r="CJ4" s="96"/>
-      <c r="CK4" s="96"/>
-      <c r="CL4" s="96"/>
-      <c r="CM4" s="96"/>
-      <c r="CN4" s="97"/>
-      <c r="CO4" s="95">
+      <c r="CI4" s="102"/>
+      <c r="CJ4" s="102"/>
+      <c r="CK4" s="102"/>
+      <c r="CL4" s="102"/>
+      <c r="CM4" s="102"/>
+      <c r="CN4" s="103"/>
+      <c r="CO4" s="101">
         <f t="shared" ref="CO4" si="4">CO5</f>
         <v>45614</v>
       </c>
-      <c r="CP4" s="96"/>
-      <c r="CQ4" s="96"/>
-      <c r="CR4" s="96"/>
-      <c r="CS4" s="96"/>
-      <c r="CT4" s="96"/>
-      <c r="CU4" s="97"/>
-      <c r="CV4" s="95">
+      <c r="CP4" s="102"/>
+      <c r="CQ4" s="102"/>
+      <c r="CR4" s="102"/>
+      <c r="CS4" s="102"/>
+      <c r="CT4" s="102"/>
+      <c r="CU4" s="103"/>
+      <c r="CV4" s="101">
         <f t="shared" ref="CV4" si="5">CV5</f>
         <v>45621</v>
       </c>
-      <c r="CW4" s="96"/>
-      <c r="CX4" s="96"/>
-      <c r="CY4" s="96"/>
-      <c r="CZ4" s="96"/>
-      <c r="DA4" s="96"/>
-      <c r="DB4" s="97"/>
-      <c r="DC4" s="95">
+      <c r="CW4" s="102"/>
+      <c r="CX4" s="102"/>
+      <c r="CY4" s="102"/>
+      <c r="CZ4" s="102"/>
+      <c r="DA4" s="102"/>
+      <c r="DB4" s="103"/>
+      <c r="DC4" s="101">
         <f t="shared" ref="DC4" si="6">DC5</f>
         <v>45628</v>
       </c>
-      <c r="DD4" s="96"/>
-      <c r="DE4" s="96"/>
-      <c r="DF4" s="96"/>
-      <c r="DG4" s="96"/>
-      <c r="DH4" s="96"/>
-      <c r="DI4" s="97"/>
-      <c r="DJ4" s="95">
+      <c r="DD4" s="102"/>
+      <c r="DE4" s="102"/>
+      <c r="DF4" s="102"/>
+      <c r="DG4" s="102"/>
+      <c r="DH4" s="102"/>
+      <c r="DI4" s="103"/>
+      <c r="DJ4" s="101">
         <f t="shared" ref="DJ4" si="7">DJ5</f>
         <v>45635</v>
       </c>
-      <c r="DK4" s="96"/>
-      <c r="DL4" s="96"/>
-      <c r="DM4" s="96"/>
-      <c r="DN4" s="96"/>
-      <c r="DO4" s="96"/>
-      <c r="DP4" s="97"/>
+      <c r="DK4" s="102"/>
+      <c r="DL4" s="102"/>
+      <c r="DM4" s="102"/>
+      <c r="DN4" s="102"/>
+      <c r="DO4" s="102"/>
+      <c r="DP4" s="103"/>
     </row>
     <row r="5" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
@@ -5467,10 +5469,10 @@
     </row>
     <row r="24" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38"/>
-      <c r="B24" s="104" t="s">
+      <c r="B24" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="95" t="s">
         <v>76</v>
       </c>
       <c r="D24" s="19">
@@ -5604,10 +5606,10 @@
     </row>
     <row r="25" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="38"/>
-      <c r="B25" s="104" t="s">
+      <c r="B25" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="101" t="s">
+      <c r="C25" s="95" t="s">
         <v>79</v>
       </c>
       <c r="D25" s="19">
@@ -5873,7 +5875,7 @@
       <c r="B27" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="102" t="s">
+      <c r="C27" s="96" t="s">
         <v>76</v>
       </c>
       <c r="D27" s="22">
@@ -6010,7 +6012,7 @@
       <c r="B28" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="102" t="s">
+      <c r="C28" s="96" t="s">
         <v>76</v>
       </c>
       <c r="D28" s="22">
@@ -6144,7 +6146,7 @@
     </row>
     <row r="29" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="38"/>
-      <c r="B29" s="103" t="s">
+      <c r="B29" s="97" t="s">
         <v>73</v>
       </c>
       <c r="C29" s="51" t="s">
@@ -6281,10 +6283,10 @@
     </row>
     <row r="30" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="38"/>
-      <c r="B30" s="103" t="s">
+      <c r="B30" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="102" t="s">
+      <c r="C30" s="96" t="s">
         <v>76</v>
       </c>
       <c r="D30" s="22">
@@ -9656,11 +9658,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="BM4:BS4"/>
     <mergeCell ref="BT4:BZ4"/>
     <mergeCell ref="BF4:BL4"/>
@@ -9669,12 +9672,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D43">
     <cfRule type="dataBar" priority="14">
@@ -9849,6 +9851,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10136,36 +10167,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10184,24 +10206,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>